<commit_message>
Small changes in the licensing results.
</commit_message>
<xml_diff>
--- a/licenses/licensing_conflicts.xlsx
+++ b/licenses/licensing_conflicts.xlsx
@@ -13335,8 +13335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added new set of manually validated clone pairs.
</commit_message>
<xml_diff>
--- a/licenses/licensing_conflicts.xlsx
+++ b/licenses/licensing_conflicts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="15540" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24940" windowHeight="14560" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="licensing_conflicts" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,10 @@
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="89" r:id="rId8"/>
-    <pivotCache cacheId="90" r:id="rId9"/>
-    <pivotCache cacheId="91" r:id="rId10"/>
-    <pivotCache cacheId="92" r:id="rId11"/>
+    <pivotCache cacheId="11" r:id="rId8"/>
+    <pivotCache cacheId="12" r:id="rId9"/>
+    <pivotCache cacheId="13" r:id="rId10"/>
+    <pivotCache cacheId="14" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11320" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11325" uniqueCount="609">
   <si>
     <t>Set</t>
   </si>
@@ -1866,6 +1866,9 @@
   </si>
   <si>
     <t>Count of SO</t>
+  </si>
+  <si>
+    <t>iReport-3.7.5-src/ireport-designer/src/com/jaspersoft/ireport/designer/subreport/TableComboBoxRenderer.java</t>
   </si>
 </sst>
 </file>
@@ -1993,6 +1996,27 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -2049,27 +2073,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10402,7 +10405,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -10659,274 +10662,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable16" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
-      <items count="42">
-        <item x="13"/>
-        <item x="26"/>
-        <item x="14"/>
-        <item x="36"/>
-        <item x="15"/>
-        <item x="37"/>
-        <item x="30"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="32"/>
-        <item x="23"/>
-        <item x="33"/>
-        <item x="2"/>
-        <item x="28"/>
-        <item x="38"/>
-        <item x="20"/>
-        <item x="31"/>
-        <item x="40"/>
-        <item x="3"/>
-        <item x="34"/>
-        <item x="4"/>
-        <item x="35"/>
-        <item x="24"/>
-        <item x="16"/>
-        <item x="39"/>
-        <item x="5"/>
-        <item x="25"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="17"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="19"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="29"/>
-        <item x="27"/>
-        <item x="18"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="42">
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Project" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="10">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="10">
-            <x v="7"/>
-            <x v="12"/>
-            <x v="18"/>
-            <x v="20"/>
-            <x v="27"/>
-            <x v="31"/>
-            <x v="32"/>
-            <x v="34"/>
-            <x v="36"/>
-            <x v="38"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="10">
-            <x v="7"/>
-            <x v="12"/>
-            <x v="18"/>
-            <x v="20"/>
-            <x v="27"/>
-            <x v="31"/>
-            <x v="32"/>
-            <x v="34"/>
-            <x v="36"/>
-            <x v="38"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="10">
-            <x v="7"/>
-            <x v="12"/>
-            <x v="18"/>
-            <x v="20"/>
-            <x v="27"/>
-            <x v="31"/>
-            <x v="32"/>
-            <x v="34"/>
-            <x v="36"/>
-            <x v="38"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable17" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable17" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:G98" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" dataField="1" showAll="0">
@@ -11336,8 +11072,275 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable16" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
+      <items count="42">
+        <item x="13"/>
+        <item x="26"/>
+        <item x="14"/>
+        <item x="36"/>
+        <item x="15"/>
+        <item x="37"/>
+        <item x="30"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="32"/>
+        <item x="23"/>
+        <item x="33"/>
+        <item x="2"/>
+        <item x="28"/>
+        <item x="38"/>
+        <item x="20"/>
+        <item x="31"/>
+        <item x="40"/>
+        <item x="3"/>
+        <item x="34"/>
+        <item x="4"/>
+        <item x="35"/>
+        <item x="24"/>
+        <item x="16"/>
+        <item x="39"/>
+        <item x="5"/>
+        <item x="25"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="17"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="29"/>
+        <item x="27"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="42">
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Project" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="10">
+            <x v="7"/>
+            <x v="12"/>
+            <x v="18"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="31"/>
+            <x v="32"/>
+            <x v="34"/>
+            <x v="36"/>
+            <x v="38"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="10">
+            <x v="7"/>
+            <x v="12"/>
+            <x v="18"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="31"/>
+            <x v="32"/>
+            <x v="34"/>
+            <x v="36"/>
+            <x v="38"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="10">
+            <x v="7"/>
+            <x v="12"/>
+            <x v="18"/>
+            <x v="20"/>
+            <x v="27"/>
+            <x v="31"/>
+            <x v="32"/>
+            <x v="34"/>
+            <x v="36"/>
+            <x v="38"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:W20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -11527,7 +11530,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable29" cacheId="92" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable29" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H314:S318" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -33692,18 +33695,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E312">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="SeeFile">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="SeeFile">
       <formula>NOT(ISERROR(SEARCH("SeeFile",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="UNKNOWN">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="UNKNOWN">
       <formula>NOT(ISERROR(SEARCH("UNKNOWN",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F230 F2:G229 F231:G312">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="SeeFile">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="SeeFile">
       <formula>NOT(ISERROR(SEARCH("SeeFile",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="UNKNOWN">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="UNKNOWN">
       <formula>NOT(ISERROR(SEARCH("UNKNOWN",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33713,10 +33716,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F400"/>
+  <dimension ref="A1:F401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B386" sqref="B386"/>
+    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="E402" sqref="E402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41689,13 +41692,30 @@
         <v>506</v>
       </c>
     </row>
+    <row r="401" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B401" t="s">
+        <v>427</v>
+      </c>
+      <c r="C401" t="s">
+        <v>535</v>
+      </c>
+      <c r="D401" t="s">
+        <v>608</v>
+      </c>
+      <c r="E401" t="s">
+        <v>8</v>
+      </c>
+      <c r="F401" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="E1:F401"/>
   <conditionalFormatting sqref="E230 E231:F313 E401:F401 E2:F229">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="SeeFile">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="SeeFile">
       <formula>NOT(ISERROR(SEARCH("SeeFile",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="UNKNOWN">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="UNKNOWN">
       <formula>NOT(ISERROR(SEARCH("UNKNOWN",E2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>